<commit_message>
Update 산출물/Architecture.png, 산출물/ERD.png, 산출물/기능 정의서.xlsx Deleted 산출물/Architecture.png, 산출물/ERD.png, 산출물/기능 정의서.xlsx
</commit_message>
<xml_diff>
--- a/산출물/기능 정의서.xlsx
+++ b/산출물/기능 정의서.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSAFY\Desktop\새 폴더\S10P12B306\산출물\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SSAFY\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t>업무대분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,26 +110,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>글을 읽어주는 TTS의 목소리를 선택할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>텍스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>동화 목록 조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>도서관</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동화 목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>등록된 동화들을 삭제할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -142,55 +126,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>부가기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>즐겨찾기 목록</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>조회</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>해당 동화에 대한 설명, 인기지수를 볼 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>책</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>저작권 만료된 음악 사용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자동재생</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>사이트를 접속하면 배경음악이 자동으로 재생됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>볼륨 조절</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>볼륨을 조절할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잠금</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>등장인물과의 대화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -199,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>생성된 이야기를 읽어줍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>재생</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,22 +151,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대화 시작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>대화 종료</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>커스텀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>내가 쓰는 동화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>대화를 다 나누면 대화를 종료할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,43 +195,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>즐겨찾기 편집</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내 책장</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이름순/최신추가순 정렬 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>동화를 다 읽으면 동화 속 등장인물을 선택해서 질문을 5번 할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>키보드나 마우스, 터치화면을 만져도 다른 기능이 작동하지 않습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>해당 동화를 내 책장에 등록할 수 있습니다. 책장에 등록하면 동화의 인기지수가 올라갑니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>한글 교육을 위해 텍스트가 노출됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>재생</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>작성한 내용을 토대로 동화 구연을 시작합니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -332,14 +240,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>재생/중지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BGM을 재생하거나 중지할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내 책장에 등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -356,18 +256,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>내 책장에 저장해서 다시 볼 수 있습니다. 다른 회원에게 공개 여부를 선택합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>다른 회원의 '나만의 동화'를 선택해 재생할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BGM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>주요 기능 안내</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -384,10 +276,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>음악</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>비회원용 메인페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -404,16 +292,183 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>슬롯 머신</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"오늘은 {아이이름}이 {주인공 이름}!" 문구를 출력합니다.
-슬롯 머신을 작동시켜 다른 주인공 이름으로 바꾸거나, 해당 동화의 재생페이지로 이동할 수 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>버튼을 통해 동화 전체 목록/내가 쓰는 동화/ 나의 책장/인기 동화 메뉴로 이동할 수 있습니다.</t>
+    <t>일반 동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름순/인기순/랜덤 정렬 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>날짜순/이름순/랜덤 정렬 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공개 여부 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 동화의 공개 여부를 수정할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼을 통해 전체 책 보기/내가 만든 동화/나의 책장으로 이동할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>친구들이 만든 최신 동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가장 최근에 다른 회원들이 만들어서 공개한 커스텀 동화 3개가 출력됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>글을 읽어주는 TTS의 목소리를 들어보고 선택할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동화 재생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성한 내용을 토대로 동화 구연을 시작합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 동화 목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 동화에 대한 인기지수를 볼 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>친구들의 동화 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생이 종료돠면 다시 만들기, 나가기, 저장할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내 책장에 저장해서 다시 볼 수 있습니다. 동화의 제목을 설정하고, 다른 회원에게 공개 여부를 선택합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>목록 조회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 회원들이 공개한 커스텀 동화의 목록을 조회할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지를 나가면 '친구들의 동화 보기'로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생이 끝나면 다른 회원들이 공개한 커스텀 동화 4개가 랜덤으로 출력됩니다. 동화를 클릭하여 재생페이지로 이동할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생이 끝나면 다시보기, 나가기를 할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등장인물과의 대화 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다시 재생, 나가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 중 한글 교육을 위해 텍스트가 노출됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스트 노출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 조절 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 중 볼륨 조절, 속도 조절, 페이지 넘김, 일시정지, 종료할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 종료 후 등장인물로부터 온 메시지가 출력됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 종료 후 재생한 동화를 다시 재생하거나 페이지를 나갈 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재생 종료 후 등장인물을 선택하여 대화를 시작할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등장인물의 메시지 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다시 재생, 나가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다시 재생, 나가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 동화 랜덤 추천</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 만든 동화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 동화와 재생 중 기능 같음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 동화와 재생 중 기능 같음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TTS를 선택하여 내가 만든 동화를 재생합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TTS를 선택하여 다른 회원들이 공개한 커스텀 동화를 재생합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지를 나가면 '전체 책 보기'로 이동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,15 +566,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -527,12 +588,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="86" zoomScaleNormal="330" zoomScaleSheetLayoutView="86" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C18" zoomScale="86" zoomScaleNormal="330" zoomScaleSheetLayoutView="86" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -825,8 +880,8 @@
     <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="120.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -851,64 +906,64 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>54</v>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -918,9 +973,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -929,9 +984,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>15</v>
       </c>
@@ -940,358 +995,468 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" t="s">
+      <c r="B17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="10"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="10"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="10"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="10"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" s="10"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" s="10"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" s="10"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" s="10"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" s="10"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" s="10"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="10"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="10"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="10"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A32" s="10"/>
+      <c r="B32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="10"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" s="10"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A35" s="10"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36" s="10"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" s="10"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" s="10"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39" s="10"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40" s="10"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41" s="9"/>
+      <c r="B41" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" s="9"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43" s="9"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44" s="9"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" t="s">
         <v>73</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E44" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A15" s="8"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A16" s="8"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A17" s="8"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A21" s="8"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A26" s="8"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A27" s="8"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A28" s="8"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32" s="7"/>
-      <c r="B32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A34" s="7"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="A13:A28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="B29:B31"/>
+  <mergeCells count="20">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B17:B31"/>
+    <mergeCell ref="B32:B40"/>
+    <mergeCell ref="A17:A40"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="C37:C40"/>
     <mergeCell ref="B2:B9"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A2:A12"/>
     <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B13:B22"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C20:C24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>